<commit_message>
fixed calcul lcr projete
</commit_message>
<xml_diff>
--- a/data/bilan.xlsx
+++ b/data/bilan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ebouafif002\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nmedia\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{470B690F-F203-432C-9E12-76C76C1F91CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821A5B3B-C194-4C5D-AB5D-27BCD62CB893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{E9D65428-2C26-42EA-949F-49ECE2CC60AB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E9D65428-2C26-42EA-949F-49ECE2CC60AB}"/>
   </bookViews>
   <sheets>
     <sheet name="BILAN" sheetId="1" r:id="rId1"/>
@@ -139,7 +139,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C38" authorId="0" shapeId="0" xr:uid="{38EF531E-5D88-482C-AD00-351DACC6DC19}">
+    <comment ref="C37" authorId="0" shapeId="0" xr:uid="{38EF531E-5D88-482C-AD00-351DACC6DC19}">
       <text>
         <r>
           <rPr>
@@ -163,7 +163,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A39" authorId="1" shapeId="0" xr:uid="{3ACEACE1-EAD0-432E-886B-CD08126207E3}">
+    <comment ref="A38" authorId="1" shapeId="0" xr:uid="{3ACEACE1-EAD0-432E-886B-CD08126207E3}">
       <text>
         <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
@@ -172,7 +172,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="D46" authorId="2" shapeId="0" xr:uid="{79F30077-17EE-4CB3-A88B-4B04B5403E33}">
+    <comment ref="D45" authorId="2" shapeId="0" xr:uid="{79F30077-17EE-4CB3-A88B-4B04B5403E33}">
       <text>
         <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
@@ -180,7 +180,7 @@
     Y compris 220 M€ de dividendes </t>
       </text>
     </comment>
-    <comment ref="D58" authorId="3" shapeId="0" xr:uid="{C1AEE366-55E6-46FA-B75B-1DA31E7E6347}">
+    <comment ref="D57" authorId="3" shapeId="0" xr:uid="{C1AEE366-55E6-46FA-B75B-1DA31E7E6347}">
       <text>
         <t>[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
@@ -193,7 +193,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="88">
   <si>
     <t>BILAN de la CMB au 30/06/2024</t>
   </si>
@@ -283,12 +283,6 @@
   </si>
   <si>
     <t>FP</t>
-  </si>
-  <si>
-    <t>Créances hypothécaires</t>
-  </si>
-  <si>
-    <t>Créances clientèle (hors hypo)</t>
   </si>
   <si>
     <r>
@@ -485,18 +479,21 @@
   <si>
     <t>Rapprochement</t>
   </si>
+  <si>
+    <t>Créances clientèle</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -633,12 +630,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1158,15 +1149,12 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="164">
+  <cellXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1183,26 +1171,8 @@
     <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1295,9 +1265,6 @@
     <xf numFmtId="3" fontId="4" fillId="3" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="10" fillId="3" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="11" fillId="3" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1335,18 +1302,9 @@
     <xf numFmtId="3" fontId="11" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="3" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="4" fillId="3" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="4" fillId="3" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1389,10 +1347,10 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="6" fillId="3" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="12" fillId="3" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1404,9 +1362,6 @@
     <xf numFmtId="3" fontId="12" fillId="3" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="10" fillId="3" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="2" fillId="3" borderId="18" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1416,7 +1371,7 @@
     <xf numFmtId="3" fontId="12" fillId="3" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="23" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="23" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="3" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1502,133 +1457,166 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="34" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="34" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="36" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="4" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="34" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="4" borderId="34" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="24" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="38" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="4" borderId="18" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="38" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="10" fillId="3" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="3" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="3" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="3" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="3" fontId="10" fillId="3" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="10" fillId="3" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="3" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="3" fontId="10" fillId="4" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="10" fillId="4" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="34" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="3" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="34" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="3" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="36" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="4" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="34" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="4" borderId="34" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="24" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="38" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="4" borderId="18" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="38" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Milliers" xfId="1" builtinId="3"/>
@@ -3844,14 +3832,14 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A39" dT="2024-10-03T14:16:27.35" personId="{D3498184-1A66-470B-88D4-42377C3DF4DF}" id="{3ACEACE1-EAD0-432E-886B-CD08126207E3}">
+  <threadedComment ref="A38" dT="2024-10-03T14:16:27.35" personId="{D3498184-1A66-470B-88D4-42377C3DF4DF}" id="{3ACEACE1-EAD0-432E-886B-CD08126207E3}">
     <text xml:space="preserve">Source corep
 </text>
   </threadedComment>
-  <threadedComment ref="D46" dT="2024-11-13T14:21:15.01" personId="{8AB6B986-D075-4EDA-9DC0-D83F10261AD7}" id="{79F30077-17EE-4CB3-A88B-4B04B5403E33}">
+  <threadedComment ref="D45" dT="2024-11-13T14:21:15.01" personId="{8AB6B986-D075-4EDA-9DC0-D83F10261AD7}" id="{79F30077-17EE-4CB3-A88B-4B04B5403E33}">
     <text xml:space="preserve">Y compris 220 M€ de dividendes </text>
   </threadedComment>
-  <threadedComment ref="D58" dT="2024-11-12T16:31:25.92" personId="{8AB6B986-D075-4EDA-9DC0-D83F10261AD7}" id="{C1AEE366-55E6-46FA-B75B-1DA31E7E6347}">
+  <threadedComment ref="D57" dT="2024-11-12T16:31:25.92" personId="{8AB6B986-D075-4EDA-9DC0-D83F10261AD7}" id="{C1AEE366-55E6-46FA-B75B-1DA31E7E6347}">
     <text>Non annulable, paiement réalisé en 2024</text>
   </threadedComment>
 </ThreadedComments>
@@ -3862,2122 +3850,2101 @@
   <sheetPr>
     <tabColor theme="3" tint="0.749992370372631"/>
   </sheetPr>
-  <dimension ref="A1:M89"/>
+  <dimension ref="A1:M88"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomRight" activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="49.7265625" style="157" customWidth="1"/>
-    <col min="2" max="2" width="21.453125" style="4" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="26.453125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.453125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="19.54296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.54296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="65.26953125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="9.81640625" style="159" customWidth="1"/>
-    <col min="9" max="9" width="12.54296875" style="159" customWidth="1"/>
-    <col min="10" max="10" width="14.54296875" style="159" customWidth="1"/>
-    <col min="11" max="11" width="19" style="159" customWidth="1"/>
-    <col min="12" max="12" width="46.7265625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="38.54296875" style="4" customWidth="1"/>
-    <col min="14" max="14" width="16.81640625" style="4" customWidth="1"/>
-    <col min="15" max="16384" width="10.81640625" style="4"/>
+    <col min="1" max="1" width="49.77734375" style="139" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" style="3" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.44140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="65.21875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="9.77734375" style="141" customWidth="1"/>
+    <col min="9" max="9" width="12.5546875" style="141" customWidth="1"/>
+    <col min="10" max="10" width="14.5546875" style="141" customWidth="1"/>
+    <col min="11" max="11" width="19" style="141" customWidth="1"/>
+    <col min="12" max="12" width="46.77734375" style="3" customWidth="1"/>
+    <col min="13" max="13" width="38.5546875" style="3" customWidth="1"/>
+    <col min="14" max="14" width="16.77734375" style="3" customWidth="1"/>
+    <col min="15" max="16384" width="10.77734375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-    </row>
-    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7" t="s">
+    <row r="1" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="148" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="148"/>
+      <c r="C1" s="148"/>
+      <c r="D1" s="148"/>
+      <c r="E1" s="148"/>
+      <c r="F1" s="148"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+    </row>
+    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="149" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="12" t="s">
+      <c r="E2" s="150"/>
+      <c r="F2" s="151"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="152" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="13"/>
-      <c r="J2" s="14" t="s">
+      <c r="I2" s="153"/>
+      <c r="J2" s="154" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="13"/>
-      <c r="L2" s="15" t="s">
+      <c r="K2" s="153"/>
+      <c r="L2" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="16" t="s">
+    <row r="3" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="J3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="21" t="s">
+      <c r="K3" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="22" t="s">
+      <c r="L3" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" s="23" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="17">
         <v>264151540.70999998</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="18">
         <v>155721823.62</v>
       </c>
-      <c r="D4" s="26">
+      <c r="D4" s="19">
         <f>D5+C4+D6</f>
         <v>156721823.62</v>
       </c>
-      <c r="E4" s="26">
+      <c r="E4" s="19">
         <f t="shared" ref="E4:F4" si="0">E5+D4+E6</f>
         <v>156721823.62</v>
       </c>
-      <c r="F4" s="26">
+      <c r="F4" s="19">
         <f t="shared" si="0"/>
         <v>156721823.62</v>
       </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" s="23"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="30">
+      <c r="G4" s="20"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="16"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="23">
         <v>1000000</v>
       </c>
-      <c r="E5" s="30">
-        <v>0</v>
-      </c>
-      <c r="F5" s="30">
-        <v>0</v>
-      </c>
-      <c r="G5" s="31"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="33"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" s="23"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="34">
+      <c r="E5" s="23">
+        <v>0</v>
+      </c>
+      <c r="F5" s="23">
+        <v>0</v>
+      </c>
+      <c r="G5" s="24"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="26"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="16"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="27">
         <f>IF([1]Paramètres!$B$12=1,-D5,0)</f>
         <v>0</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="27">
         <f t="shared" ref="E6:F6" si="1">-E5</f>
         <v>0</v>
       </c>
-      <c r="F6" s="34">
+      <c r="F6" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G6" s="31"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="33"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" s="36" t="s">
+      <c r="G6" s="24"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="26"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="24">
+      <c r="B7" s="17">
         <v>4753518315.8799992</v>
       </c>
-      <c r="C7" s="37">
+      <c r="C7" s="30">
         <v>4191260525.8000002</v>
       </c>
-      <c r="D7" s="37">
+      <c r="D7" s="30">
         <f>C7+D8+D9+Retrait_depôts_stress_2025_Créance_CMB+D11+D12</f>
         <v>4388260525.8000002</v>
       </c>
-      <c r="E7" s="37">
+      <c r="E7" s="30">
         <f>D7+E8+E9+Retrait_depôts_stress_2026_Créance_CMB+E11+E12</f>
         <v>4698560525.8000002</v>
       </c>
-      <c r="F7" s="37">
+      <c r="F7" s="30">
         <f>E7+F8+F9+Retrait_depôts_stress_2027_Créance_CMB+F11+F12</f>
         <v>4897060525.8000002</v>
       </c>
-      <c r="G7" s="38"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39"/>
-      <c r="K7" s="39"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" s="40"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="30">
+      <c r="G7" s="31"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="33"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="23">
         <v>197000000</v>
       </c>
-      <c r="E8" s="30">
+      <c r="E8" s="23">
         <v>310300000</v>
       </c>
-      <c r="F8" s="30">
+      <c r="F8" s="23">
         <v>198500000</v>
       </c>
-      <c r="G8" s="31" t="s">
+      <c r="G8" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-    </row>
-    <row r="9" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="40"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="42">
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+    </row>
+    <row r="9" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="33"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="35">
         <f>IF([1]Paramètres!$B$12=1,-D8,0)</f>
         <v>0</v>
       </c>
-      <c r="E9" s="42">
+      <c r="E9" s="35">
         <f>IF([1]Paramètres!$B$12=1,-E8,0)</f>
         <v>0</v>
       </c>
-      <c r="F9" s="42">
+      <c r="F9" s="35">
         <f>IF([1]Paramètres!$B$12=1,-F8,0)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="43" t="s">
+      <c r="G9" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="44"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A10" s="40"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="34">
-        <f>D56*[1]Paramètres!$B$4</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="34">
-        <f>E56*[1]Paramètres!$B$4</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="34">
-        <f>F56*[1]Paramètres!$B$4</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="43" t="s">
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="33"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="27">
+        <f>D55*[1]Paramètres!$B$4</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="27">
+        <f>E55*[1]Paramètres!$B$4</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="27">
+        <f>F55*[1]Paramètres!$B$4</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="44" t="s">
+      <c r="H10" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="44" t="s">
+      <c r="I10" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="J10" s="44" t="s">
+      <c r="J10" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="K10" s="44" t="s">
+      <c r="K10" s="37" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" s="40"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="34">
-        <f>D50*[1]Paramètres!$E$13</f>
-        <v>0</v>
-      </c>
-      <c r="E11" s="34">
-        <f>E50*[1]Paramètres!$E$13</f>
-        <v>0</v>
-      </c>
-      <c r="F11" s="34">
-        <f>F50*[1]Paramètres!$E$13</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="43" t="s">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="33"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="27">
+        <f>D49*[1]Paramètres!$E$13</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="27">
+        <f>E49*[1]Paramètres!$E$13</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="27">
+        <f>F49*[1]Paramètres!$E$13</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="H11" s="44" t="s">
+      <c r="H11" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="44" t="s">
+      <c r="I11" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="J11" s="44" t="s">
+      <c r="J11" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="44" t="s">
+      <c r="K11" s="37" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12" s="45"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="34">
-        <f>SUM(D71:D73)</f>
-        <v>0</v>
-      </c>
-      <c r="E12" s="34">
-        <f t="shared" ref="E12:F12" si="2">SUM(E71:E73)</f>
-        <v>0</v>
-      </c>
-      <c r="F12" s="34">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="38"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="27">
+        <f>SUM(D70:D72)</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="27">
+        <f t="shared" ref="E12:F12" si="2">SUM(E70:E72)</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="27">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G12" s="43" t="s">
+      <c r="G12" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="H12" s="44" t="s">
+      <c r="H12" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="I12" s="44" t="s">
+      <c r="I12" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="J12" s="44" t="s">
+      <c r="J12" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="K12" s="44" t="s">
+      <c r="K12" s="37" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A13" s="45" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="19">
+        <v>865980732.12</v>
+      </c>
+      <c r="C13" s="146">
+        <v>2896774257.4000001</v>
+      </c>
+      <c r="D13" s="146">
+        <f>C13+D14+D15+D16+D17+D18</f>
+        <v>3204774257.4000001</v>
+      </c>
+      <c r="E13" s="146">
+        <f>D13+E14+E15+E16+E17+E18</f>
+        <v>3554774257.4000001</v>
+      </c>
+      <c r="F13" s="146">
+        <f>E13+F14+F15+F16+F17+F18</f>
+        <v>3904774257.4000001</v>
+      </c>
+      <c r="G13" s="39"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="40"/>
+    </row>
+    <row r="14" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="41"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="23">
+        <v>308000000</v>
+      </c>
+      <c r="E14" s="23">
+        <v>350000000</v>
+      </c>
+      <c r="F14" s="23">
+        <v>350000000</v>
+      </c>
+      <c r="G14" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="26">
-        <v>865980732.12</v>
-      </c>
-      <c r="C13" s="46">
-        <v>2896774257.4000001</v>
-      </c>
-      <c r="D13" s="46">
-        <f>C13+D15+D16+D17+D18+D19</f>
-        <v>3204774257.4000001</v>
-      </c>
-      <c r="E13" s="46">
-        <f>D13+E15+E16+E17+E18+E19</f>
-        <v>3554774257.4000001</v>
-      </c>
-      <c r="F13" s="46">
-        <f>E13+F15+F16+F17+F18+F19</f>
-        <v>3904774257.4000001</v>
-      </c>
-      <c r="G13" s="47"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="48"/>
-      <c r="K13" s="48"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A14" s="49" t="s">
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="33"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="44">
+        <f>IF([1]Paramètres!$B$12=1,-D14,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="44">
+        <f>IF([1]Paramètres!$B$12=1,-E14,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="44">
+        <f>IF([1]Paramètres!$B$12=1,-F14,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="26">
-        <v>2074968405.6800003</v>
-      </c>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="48"/>
-      <c r="K14" s="48"/>
-    </row>
-    <row r="15" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="49"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="30">
-        <v>308000000</v>
-      </c>
-      <c r="E15" s="30">
-        <v>350000000</v>
-      </c>
-      <c r="F15" s="30">
-        <v>350000000</v>
-      </c>
-      <c r="G15" s="31" t="s">
+      <c r="H15" s="45"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="45"/>
+      <c r="K15" s="45"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="33"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="44">
+        <f>($C$37*[1]Paramètres!$H$3)/3</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="44">
+        <f>($C$37*[1]Paramètres!$H$3)/3</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="44">
+        <f>($C$37*[1]Paramètres!$H$3)/3</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A16" s="40"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="52">
-        <f>IF([1]Paramètres!$B$12=1,-D15,0)</f>
-        <v>0</v>
-      </c>
-      <c r="E16" s="52">
-        <f>IF([1]Paramètres!$B$12=1,-E15,0)</f>
-        <v>0</v>
-      </c>
-      <c r="F16" s="52">
-        <f>IF([1]Paramètres!$B$12=1,-F15,0)</f>
-        <v>0</v>
-      </c>
-      <c r="G16" s="43" t="s">
+      <c r="H16" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="J16" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="K16" s="45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="33"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="44">
+        <f>D75</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="44">
+        <f>E75</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="44">
+        <f>F75</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="H16" s="53"/>
-      <c r="I16" s="53"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="53"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17" s="40"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="51"/>
-      <c r="D17" s="52">
-        <f>($C$38*[1]Paramètres!$H$3)/3</f>
-        <v>0</v>
-      </c>
-      <c r="E17" s="52">
-        <f>($C$38*[1]Paramètres!$H$3)/3</f>
-        <v>0</v>
-      </c>
-      <c r="F17" s="52">
-        <f>($C$38*[1]Paramètres!$H$3)/3</f>
-        <v>0</v>
-      </c>
-      <c r="G17" s="43" t="s">
+      <c r="H17" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="48"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="38"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="44">
+        <f>-[1]Paramètres!E33</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="H17" s="53" t="s">
+      <c r="H18" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="I17" s="53" t="s">
+      <c r="I18" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="J17" s="53" t="s">
+      <c r="J18" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="K17" s="53" t="s">
+      <c r="K18" s="45" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A18" s="40"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="52">
-        <f>D76</f>
-        <v>0</v>
-      </c>
-      <c r="E18" s="52">
-        <f>E76</f>
-        <v>0</v>
-      </c>
-      <c r="F18" s="52">
-        <f>F76</f>
-        <v>0</v>
-      </c>
-      <c r="G18" s="54" t="s">
+      <c r="L18" s="48"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="H18" s="44" t="s">
+      <c r="B19" s="18">
+        <v>809704829.41999984</v>
+      </c>
+      <c r="C19" s="18">
+        <v>863578713.20000005</v>
+      </c>
+      <c r="D19" s="18">
+        <f>C19+D20+D21+D22+D23+D24+D25+D27+D26</f>
+        <v>744578713.20000005</v>
+      </c>
+      <c r="E19" s="18">
+        <f>D19+E20+E21+E22+E23+E24+E25+E27+E26</f>
+        <v>618278713.19999993</v>
+      </c>
+      <c r="F19" s="18">
+        <f>E19+F20+F21+F22+F23+F24+F25+F27+F26</f>
+        <v>614778713.19999993</v>
+      </c>
+      <c r="G19" s="50"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="155"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="23">
+        <v>-119000000</v>
+      </c>
+      <c r="E20" s="23">
+        <v>-126300000.00000012</v>
+      </c>
+      <c r="F20" s="23">
+        <v>-3500000</v>
+      </c>
+      <c r="G20" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="52"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="156"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="44">
+        <f>IF([1]Paramètres!$B$12=1,-D20,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="44">
+        <f>IF([1]Paramètres!$B$12=1,-E20,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="44">
+        <f>IF([1]Paramètres!$B$12=1,-F20,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="H21" s="45"/>
+      <c r="I21" s="45"/>
+      <c r="J21" s="45"/>
+      <c r="K21" s="45"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="156"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="44">
+        <f>D55*[1]Paramètres!$B$5</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="44">
+        <f>E55*[1]Paramètres!$B$5</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="44">
+        <f>F55*[1]Paramètres!$B$5</f>
+        <v>0</v>
+      </c>
+      <c r="G22" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="I18" s="55" t="s">
-        <v>24</v>
-      </c>
-      <c r="J18" s="55"/>
-      <c r="K18" s="55"/>
-      <c r="L18" s="56"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A19" s="45"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="51"/>
-      <c r="D19" s="52">
-        <f>-[1]Paramètres!E33</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="52"/>
-      <c r="F19" s="52"/>
-      <c r="G19" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="H19" s="44" t="s">
+      <c r="I22" s="37"/>
+      <c r="J22" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="K22" s="37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="156"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="44">
+        <f>-($C$19*[1]Paramètres!$K$3*[1]Paramètres!$K$4)/3</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="44">
+        <f>-($C$19*[1]Paramètres!$K$3*[1]Paramètres!$K$4)/3</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="44">
+        <f>-($C$19*[1]Paramètres!$K$3*[1]Paramètres!$K$4)/3</f>
+        <v>0</v>
+      </c>
+      <c r="G23" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="H23" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="I19" s="55" t="s">
-        <v>24</v>
-      </c>
-      <c r="J19" s="53" t="s">
+      <c r="I23" s="37"/>
+      <c r="J23" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="K23" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="L23" s="53"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="156"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="44">
+        <f>-($C$19*[1]Paramètres!$K$3*[1]Paramètres!$K$5)/3</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="44">
+        <f>-($C$19*[1]Paramètres!$K$3*[1]Paramètres!$K$5)/3</f>
+        <v>0</v>
+      </c>
+      <c r="F24" s="44">
+        <f>-($C$19*[1]Paramètres!$K$3*[1]Paramètres!$K$5)/3</f>
+        <v>0</v>
+      </c>
+      <c r="G24" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="H24" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="I24" s="37"/>
+      <c r="J24" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="K19" s="53" t="s">
+      <c r="K24" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="L19" s="56"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A20" s="57" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="25">
-        <v>809704829.41999984</v>
-      </c>
-      <c r="C20" s="25">
-        <v>863578713.20000005</v>
-      </c>
-      <c r="D20" s="25">
-        <f>C20+D21+D22+D23+D24+D25+D26+D28+D27</f>
-        <v>744578713.20000005</v>
-      </c>
-      <c r="E20" s="25">
-        <f>D20+E21+E22+E23+E24+E25+E26+E28+E27</f>
-        <v>618278713.19999993</v>
-      </c>
-      <c r="F20" s="25">
-        <f>E20+F21+F22+F23+F24+F25+F26+F28+F27</f>
-        <v>614778713.19999993</v>
-      </c>
-      <c r="G20" s="58"/>
-      <c r="H20" s="59"/>
-      <c r="I20" s="59"/>
-      <c r="J20" s="59"/>
-      <c r="K20" s="59"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A21" s="60"/>
-      <c r="B21" s="29"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="30">
-        <v>-119000000</v>
-      </c>
-      <c r="E21" s="30">
-        <v>-126300000.00000012</v>
-      </c>
-      <c r="F21" s="30">
-        <v>-3500000</v>
-      </c>
-      <c r="G21" s="31" t="s">
+      <c r="L24" s="54"/>
+    </row>
+    <row r="25" spans="1:13" ht="29.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="156"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="44">
+        <f>D16*(-[1]Paramètres!$H$8)</f>
+        <v>0</v>
+      </c>
+      <c r="E25" s="44">
+        <f>E16*(-[1]Paramètres!$H$8)</f>
+        <v>0</v>
+      </c>
+      <c r="F25" s="44">
+        <f>F16*(-[1]Paramètres!$H$8)</f>
+        <v>0</v>
+      </c>
+      <c r="G25" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="H25" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="I25" s="45"/>
+      <c r="J25" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
-      <c r="K21" s="32"/>
-      <c r="L21" s="61"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A22" s="62"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="52">
-        <f>IF([1]Paramètres!$B$12=1,-D21,0)</f>
-        <v>0</v>
-      </c>
-      <c r="E22" s="52">
-        <f>IF([1]Paramètres!$B$12=1,-E21,0)</f>
-        <v>0</v>
-      </c>
-      <c r="F22" s="52">
-        <f>IF([1]Paramètres!$B$12=1,-F21,0)</f>
-        <v>0</v>
-      </c>
-      <c r="G22" s="43" t="s">
+      <c r="K25" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="H22" s="53"/>
-      <c r="I22" s="53"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="53"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A23" s="62"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="52">
-        <f>D56*[1]Paramètres!$B$5</f>
-        <v>0</v>
-      </c>
-      <c r="E23" s="52">
-        <f>E56*[1]Paramètres!$B$5</f>
-        <v>0</v>
-      </c>
-      <c r="F23" s="52">
-        <f>F56*[1]Paramètres!$B$5</f>
-        <v>0</v>
-      </c>
-      <c r="G23" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="H23" s="44" t="s">
+      <c r="M25" s="52"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="156"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="44">
+        <f>D49*[1]Paramètres!$E$14</f>
+        <v>0</v>
+      </c>
+      <c r="E26" s="44">
+        <f>E49*[1]Paramètres!$E$14</f>
+        <v>0</v>
+      </c>
+      <c r="F26" s="44">
+        <f>F49*[1]Paramètres!$E$14</f>
+        <v>0</v>
+      </c>
+      <c r="G26" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="H26" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="I23" s="44"/>
-      <c r="J23" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="K23" s="44" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A24" s="62"/>
-      <c r="B24" s="29"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="52">
-        <f>-($C$20*[1]Paramètres!$K$3*[1]Paramètres!$K$4)/3</f>
-        <v>0</v>
-      </c>
-      <c r="E24" s="52">
-        <f>-($C$20*[1]Paramètres!$K$3*[1]Paramètres!$K$4)/3</f>
-        <v>0</v>
-      </c>
-      <c r="F24" s="52">
-        <f>-($C$20*[1]Paramètres!$K$3*[1]Paramètres!$K$4)/3</f>
-        <v>0</v>
-      </c>
-      <c r="G24" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="H24" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="I24" s="44"/>
-      <c r="J24" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="K24" s="44" t="s">
-        <v>41</v>
-      </c>
-      <c r="L24" s="63"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A25" s="62"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="52">
-        <f>-($C$20*[1]Paramètres!$K$3*[1]Paramètres!$K$5)/3</f>
-        <v>0</v>
-      </c>
-      <c r="E25" s="52">
-        <f>-($C$20*[1]Paramètres!$K$3*[1]Paramètres!$K$5)/3</f>
-        <v>0</v>
-      </c>
-      <c r="F25" s="52">
-        <f>-($C$20*[1]Paramètres!$K$3*[1]Paramètres!$K$5)/3</f>
-        <v>0</v>
-      </c>
-      <c r="G25" s="43" t="s">
+      <c r="I26" s="37"/>
+      <c r="J26" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="K26" s="37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="157"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="44">
+        <f>-([1]Paramètres!$K$30*[1]C7200_TOTAL_HQLA!$D$16)/3</f>
+        <v>0</v>
+      </c>
+      <c r="E27" s="44">
+        <f>-([1]Paramètres!$K$30*[1]C7200_TOTAL_HQLA!$D$16)/3</f>
+        <v>0</v>
+      </c>
+      <c r="F27" s="44">
+        <f>-([1]Paramètres!$K$30*[1]C7200_TOTAL_HQLA!$D$16)/3</f>
+        <v>0</v>
+      </c>
+      <c r="G27" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="H25" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="I25" s="44"/>
-      <c r="J25" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="K25" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="L25" s="64"/>
-    </row>
-    <row r="26" spans="1:13" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="62"/>
-      <c r="B26" s="29"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="52">
-        <f>D17*(-[1]Paramètres!$H$8)</f>
-        <v>0</v>
-      </c>
-      <c r="E26" s="52">
-        <f>E17*(-[1]Paramètres!$H$8)</f>
-        <v>0</v>
-      </c>
-      <c r="F26" s="52">
-        <f>F17*(-[1]Paramètres!$H$8)</f>
-        <v>0</v>
-      </c>
-      <c r="G26" s="43" t="s">
+      <c r="H27" s="45"/>
+      <c r="I27" s="45"/>
+      <c r="J27" s="55"/>
+      <c r="K27" s="56"/>
+      <c r="L27" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="H26" s="53" t="s">
-        <v>23</v>
-      </c>
-      <c r="I26" s="53"/>
-      <c r="J26" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="K26" s="44" t="s">
-        <v>41</v>
-      </c>
-      <c r="M26" s="61"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A27" s="62"/>
-      <c r="B27" s="29"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="52">
-        <f>D50*[1]Paramètres!$E$14</f>
-        <v>0</v>
-      </c>
-      <c r="E27" s="52">
-        <f>E50*[1]Paramètres!$E$14</f>
-        <v>0</v>
-      </c>
-      <c r="F27" s="52">
-        <f>F50*[1]Paramètres!$E$14</f>
-        <v>0</v>
-      </c>
-      <c r="G27" s="43" t="s">
-        <v>27</v>
-      </c>
-      <c r="H27" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="I27" s="44"/>
-      <c r="J27" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="K27" s="44" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A28" s="65"/>
-      <c r="B28" s="29"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="52">
-        <f>-([1]Paramètres!$K$30*[1]C7200_TOTAL_HQLA!$D$16)/3</f>
-        <v>0</v>
-      </c>
-      <c r="E28" s="52">
-        <f>-([1]Paramètres!$K$30*[1]C7200_TOTAL_HQLA!$D$16)/3</f>
-        <v>0</v>
-      </c>
-      <c r="F28" s="52">
-        <f>-([1]Paramètres!$K$30*[1]C7200_TOTAL_HQLA!$D$16)/3</f>
-        <v>0</v>
-      </c>
-      <c r="G28" s="43" t="s">
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="H28" s="53"/>
-      <c r="I28" s="53"/>
-      <c r="J28" s="66"/>
-      <c r="K28" s="67"/>
-      <c r="L28" s="68" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A29" s="69" t="s">
-        <v>47</v>
-      </c>
-      <c r="B29" s="26">
+      <c r="B28" s="19">
         <v>55739716.989999995</v>
       </c>
-      <c r="C29" s="70">
+      <c r="C28" s="59">
         <v>2348229.34</v>
       </c>
-      <c r="D29" s="70">
-        <f>$C$29</f>
+      <c r="D28" s="59">
+        <f>$C$28</f>
         <v>2348229.34</v>
       </c>
-      <c r="E29" s="70">
-        <f t="shared" ref="E29:F29" si="3">$C$29</f>
+      <c r="E28" s="59">
+        <f t="shared" ref="E28:F28" si="3">$C$28</f>
         <v>2348229.34</v>
       </c>
-      <c r="F29" s="70">
+      <c r="F28" s="59">
         <f t="shared" si="3"/>
         <v>2348229.34</v>
       </c>
-      <c r="G29" s="31"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="71"/>
-      <c r="K29" s="32"/>
-      <c r="L29" s="72"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A30" s="73" t="s">
+      <c r="G28" s="24"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="60"/>
+      <c r="K28" s="25"/>
+      <c r="L28" s="61"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="62" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="19">
+        <v>235377564.62000763</v>
+      </c>
+      <c r="C29" s="19">
+        <v>228174947.12999997</v>
+      </c>
+      <c r="D29" s="19">
+        <f>C29+D30+D31+D32+D33+D34</f>
+        <v>334174947.13</v>
+      </c>
+      <c r="E29" s="19">
+        <f>D29+E30+E31+E32+E33+E34</f>
+        <v>372174947.13</v>
+      </c>
+      <c r="F29" s="19">
+        <f>E29+F30+F31+F32+F33+F34</f>
+        <v>462174947.13</v>
+      </c>
+      <c r="G29" s="39"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="60"/>
+      <c r="K29" s="40"/>
+      <c r="L29" s="63"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" s="64"/>
+      <c r="B30" s="65"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="23">
+        <v>106000000</v>
+      </c>
+      <c r="E30" s="23">
+        <v>38000000</v>
+      </c>
+      <c r="F30" s="23">
+        <v>90000000</v>
+      </c>
+      <c r="G30" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="H30" s="25"/>
+      <c r="I30" s="25"/>
+      <c r="J30" s="60"/>
+      <c r="K30" s="25"/>
+      <c r="L30" s="61"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="64"/>
+      <c r="B31" s="65"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="35">
+        <f>IF([1]Paramètres!$B$12=1,-D30,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="35">
+        <f>IF([1]Paramètres!$B$12=1,-E30,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="35">
+        <f>IF([1]Paramètres!$B$12=1,-F30,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G31" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="26">
-        <v>235377564.62000763</v>
-      </c>
-      <c r="C30" s="26">
-        <v>228174947.12999997</v>
-      </c>
-      <c r="D30" s="26">
-        <f>C30+D31+D32+D33+D34+D35</f>
-        <v>334174947.13</v>
-      </c>
-      <c r="E30" s="26">
-        <f>D30+E31+E32+E33+E34+E35</f>
-        <v>372174947.13</v>
-      </c>
-      <c r="F30" s="26">
-        <f>E30+F31+F32+F33+F34+F35</f>
-        <v>462174947.13</v>
-      </c>
-      <c r="G30" s="47"/>
-      <c r="H30" s="48"/>
-      <c r="I30" s="48"/>
-      <c r="J30" s="71"/>
-      <c r="K30" s="48"/>
-      <c r="L30" s="74"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A31" s="75"/>
-      <c r="B31" s="76"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="30">
-        <v>106000000</v>
-      </c>
-      <c r="E31" s="30">
-        <v>38000000</v>
-      </c>
-      <c r="F31" s="30">
-        <v>90000000</v>
-      </c>
-      <c r="G31" s="31" t="s">
+      <c r="H31" s="45"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="45"/>
+      <c r="K31" s="66"/>
+      <c r="L31" s="52"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" s="64"/>
+      <c r="B32" s="65"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="67">
+        <f>D73</f>
+        <v>0</v>
+      </c>
+      <c r="E32" s="67">
+        <f t="shared" ref="E32:F33" si="4">E73</f>
+        <v>0</v>
+      </c>
+      <c r="F32" s="67">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G32" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="H31" s="32"/>
-      <c r="I31" s="32"/>
-      <c r="J31" s="71"/>
-      <c r="K31" s="32"/>
-      <c r="L31" s="72"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A32" s="75"/>
-      <c r="B32" s="76"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="42">
-        <f>IF([1]Paramètres!$B$12=1,-D31,0)</f>
-        <v>0</v>
-      </c>
-      <c r="E32" s="42">
-        <f>IF([1]Paramètres!$B$12=1,-E31,0)</f>
-        <v>0</v>
-      </c>
-      <c r="F32" s="42">
-        <f>IF([1]Paramètres!$B$12=1,-F31,0)</f>
-        <v>0</v>
-      </c>
-      <c r="G32" s="43" t="s">
+      <c r="H32" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="I32" s="37"/>
+      <c r="J32" s="45"/>
+      <c r="K32" s="45"/>
+      <c r="L32" s="52"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" s="64"/>
+      <c r="B33" s="65"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="67">
+        <f>D74</f>
+        <v>0</v>
+      </c>
+      <c r="E33" s="67">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F33" s="67">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G33" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="H32" s="53"/>
-      <c r="I32" s="53"/>
-      <c r="J32" s="53"/>
-      <c r="K32" s="77"/>
-      <c r="L32" s="61"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A33" s="75"/>
-      <c r="B33" s="76"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="78">
-        <f>D74</f>
-        <v>0</v>
-      </c>
-      <c r="E33" s="78">
-        <f t="shared" ref="E33:F34" si="4">E74</f>
-        <v>0</v>
-      </c>
-      <c r="F33" s="78">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G33" s="43" t="s">
+      <c r="H33" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="I33" s="37"/>
+      <c r="J33" s="45"/>
+      <c r="K33" s="45"/>
+      <c r="L33" s="52"/>
+    </row>
+    <row r="34" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="64"/>
+      <c r="B34" s="65"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="67">
+        <f>D77</f>
+        <v>0</v>
+      </c>
+      <c r="E34" s="67">
+        <f t="shared" ref="E34:F34" si="5">E77</f>
+        <v>0</v>
+      </c>
+      <c r="F34" s="67">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G34" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="H33" s="53" t="s">
+      <c r="H34" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="I33" s="44"/>
-      <c r="J33" s="53"/>
-      <c r="K33" s="53"/>
-      <c r="L33" s="61"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A34" s="75"/>
-      <c r="B34" s="76"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="78">
-        <f>D75</f>
-        <v>0</v>
-      </c>
-      <c r="E34" s="78">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F34" s="78">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G34" s="43" t="s">
+      <c r="I34" s="45"/>
+      <c r="J34" s="45"/>
+      <c r="K34" s="37"/>
+    </row>
+    <row r="35" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="69">
+        <f>SUM(B4:B29)</f>
+        <v>6984472699.7400064</v>
+      </c>
+      <c r="C35" s="70">
+        <v>8337858496.4899998</v>
+      </c>
+      <c r="D35" s="70">
+        <f>SUM(D4,D7,D13,D19,D28,D29)</f>
+        <v>8830858496.4899998</v>
+      </c>
+      <c r="E35" s="70">
+        <f>SUM(E4,E7,E13,E19,E28,E29)</f>
+        <v>9402858496.4899998</v>
+      </c>
+      <c r="F35" s="70">
+        <f>SUM(F4,F7,F13,F19,F28,F29)</f>
+        <v>10037858496.49</v>
+      </c>
+      <c r="G35" s="71"/>
+      <c r="H35" s="72"/>
+      <c r="I35" s="72"/>
+      <c r="J35" s="72"/>
+      <c r="K35" s="73"/>
+    </row>
+    <row r="36" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="38"/>
+      <c r="B36" s="42"/>
+      <c r="C36" s="74"/>
+      <c r="D36" s="74"/>
+      <c r="E36" s="74"/>
+      <c r="F36" s="74"/>
+      <c r="G36" s="75"/>
+      <c r="H36" s="76"/>
+      <c r="I36" s="76"/>
+      <c r="J36" s="76"/>
+      <c r="K36" s="76"/>
+    </row>
+    <row r="37" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="68" t="s">
         <v>52</v>
       </c>
-      <c r="H34" s="53" t="s">
-        <v>23</v>
-      </c>
-      <c r="I34" s="44"/>
-      <c r="J34" s="53"/>
-      <c r="K34" s="53"/>
-      <c r="L34" s="61"/>
-    </row>
-    <row r="35" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="75"/>
-      <c r="B35" s="76"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="78">
-        <f>D78</f>
-        <v>0</v>
-      </c>
-      <c r="E35" s="78">
-        <f t="shared" ref="E35:F35" si="5">E78</f>
-        <v>0</v>
-      </c>
-      <c r="F35" s="78">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G35" s="43" t="s">
+      <c r="B37" s="19">
+        <v>1039163376.0900002</v>
+      </c>
+      <c r="C37" s="77">
+        <v>1293887720.8</v>
+      </c>
+      <c r="D37" s="78">
+        <f>C37</f>
+        <v>1293887720.8</v>
+      </c>
+      <c r="E37" s="78">
+        <f>D37</f>
+        <v>1293887720.8</v>
+      </c>
+      <c r="F37" s="78">
+        <f>E37</f>
+        <v>1293887720.8</v>
+      </c>
+      <c r="G37" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="H35" s="53" t="s">
-        <v>23</v>
-      </c>
-      <c r="I35" s="53"/>
-      <c r="J35" s="53"/>
-      <c r="K35" s="44"/>
-    </row>
-    <row r="36" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="79" t="s">
-        <v>23</v>
-      </c>
-      <c r="B36" s="80">
-        <f>SUM(B4:B30)</f>
-        <v>9059441105.4200077</v>
-      </c>
-      <c r="C36" s="81">
-        <v>8337858496.4899998</v>
-      </c>
-      <c r="D36" s="81">
-        <f>SUM(D4,D7,D13,D20,D29,D30)</f>
-        <v>8830858496.4899998</v>
-      </c>
-      <c r="E36" s="81">
-        <f>SUM(E4,E7,E13,E20,E29,E30)</f>
-        <v>9402858496.4899998</v>
-      </c>
-      <c r="F36" s="81">
-        <f>SUM(F4,F7,F13,F20,F29,F30)</f>
-        <v>10037858496.49</v>
-      </c>
-      <c r="G36" s="82"/>
-      <c r="H36" s="83"/>
-      <c r="I36" s="83"/>
-      <c r="J36" s="83"/>
-      <c r="K36" s="84"/>
-    </row>
-    <row r="37" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="45"/>
-      <c r="B37" s="85"/>
-      <c r="C37" s="86"/>
-      <c r="D37" s="86"/>
-      <c r="E37" s="86"/>
-      <c r="F37" s="86"/>
-      <c r="G37" s="87"/>
-      <c r="H37" s="88"/>
-      <c r="I37" s="88"/>
-      <c r="J37" s="88"/>
-      <c r="K37" s="88"/>
-    </row>
-    <row r="38" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H37" s="25"/>
+      <c r="I37" s="25"/>
+      <c r="J37" s="25"/>
+      <c r="K37" s="25"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="79" t="s">
         <v>54</v>
       </c>
-      <c r="B38" s="26">
-        <v>1039163376.0900002</v>
-      </c>
-      <c r="C38" s="89">
-        <v>1293887720.8</v>
-      </c>
-      <c r="D38" s="90">
-        <f>C38</f>
-        <v>1293887720.8</v>
-      </c>
-      <c r="E38" s="90">
-        <f>D38</f>
-        <v>1293887720.8</v>
-      </c>
-      <c r="F38" s="90">
-        <f>E38</f>
-        <v>1293887720.8</v>
-      </c>
-      <c r="G38" s="31" t="s">
+      <c r="B38" s="80"/>
+      <c r="C38" s="78">
+        <v>814573537.46000004</v>
+      </c>
+      <c r="D38" s="81"/>
+      <c r="E38" s="81"/>
+      <c r="F38" s="81"/>
+      <c r="G38" s="82"/>
+      <c r="H38" s="61"/>
+      <c r="I38" s="61"/>
+      <c r="J38" s="61"/>
+      <c r="K38" s="61"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39" s="79" t="s">
         <v>55</v>
       </c>
-      <c r="H38" s="32"/>
-      <c r="I38" s="32"/>
-      <c r="J38" s="32"/>
-      <c r="K38" s="32"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A39" s="91" t="s">
+      <c r="B39" s="80"/>
+      <c r="C39" s="78">
+        <v>442549090.30000001</v>
+      </c>
+      <c r="D39" s="81"/>
+      <c r="E39" s="81"/>
+      <c r="F39" s="81"/>
+      <c r="G39" s="82"/>
+      <c r="H39" s="61"/>
+      <c r="I39" s="61"/>
+      <c r="J39" s="61"/>
+      <c r="K39" s="61"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A40" s="79" t="s">
         <v>56</v>
       </c>
-      <c r="B39" s="92"/>
-      <c r="C39" s="90">
-        <v>814573537.46000004</v>
-      </c>
-      <c r="D39" s="93"/>
-      <c r="E39" s="93"/>
-      <c r="F39" s="93"/>
-      <c r="G39" s="94"/>
-      <c r="H39" s="72"/>
-      <c r="I39" s="72"/>
-      <c r="J39" s="72"/>
-      <c r="K39" s="72"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A40" s="91" t="s">
+      <c r="B40" s="80"/>
+      <c r="C40" s="78">
+        <v>36045189.469999999</v>
+      </c>
+      <c r="D40" s="81"/>
+      <c r="E40" s="81"/>
+      <c r="F40" s="81"/>
+      <c r="G40" s="82"/>
+      <c r="H40" s="61"/>
+      <c r="I40" s="61"/>
+      <c r="J40" s="61"/>
+      <c r="K40" s="61"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41" s="83" t="s">
         <v>57</v>
       </c>
-      <c r="B40" s="92"/>
-      <c r="C40" s="90">
-        <v>442549090.30000001</v>
-      </c>
-      <c r="D40" s="93"/>
-      <c r="E40" s="93"/>
-      <c r="F40" s="93"/>
-      <c r="G40" s="94"/>
-      <c r="H40" s="72"/>
-      <c r="I40" s="72"/>
-      <c r="J40" s="72"/>
-      <c r="K40" s="72"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A41" s="91" t="s">
+      <c r="B41" s="84"/>
+      <c r="C41" s="84"/>
+      <c r="D41" s="84"/>
+      <c r="E41" s="84"/>
+      <c r="F41" s="84"/>
+      <c r="G41" s="84"/>
+      <c r="H41" s="85"/>
+      <c r="I41" s="85"/>
+      <c r="J41" s="85"/>
+      <c r="K41" s="85"/>
+    </row>
+    <row r="43" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A43" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B41" s="92"/>
-      <c r="C41" s="90">
-        <v>36045189.469999999</v>
-      </c>
-      <c r="D41" s="93"/>
-      <c r="E41" s="93"/>
-      <c r="F41" s="93"/>
-      <c r="G41" s="94"/>
-      <c r="H41" s="72"/>
-      <c r="I41" s="72"/>
-      <c r="J41" s="72"/>
-      <c r="K41" s="72"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A42" s="95" t="s">
+      <c r="B43" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G43" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H43" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I43" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J43" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="K43" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44" s="86" t="s">
         <v>59</v>
       </c>
-      <c r="B42" s="96"/>
-      <c r="C42" s="96"/>
-      <c r="D42" s="96"/>
-      <c r="E42" s="96"/>
-      <c r="F42" s="96"/>
-      <c r="G42" s="96"/>
-      <c r="H42" s="97"/>
-      <c r="I42" s="97"/>
-      <c r="J42" s="97"/>
-      <c r="K42" s="97"/>
-    </row>
-    <row r="44" spans="1:12" ht="17" x14ac:dyDescent="0.35">
-      <c r="A44" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="B44" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C44" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D44" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E44" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="F44" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="G44" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="H44" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="I44" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="J44" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="K44" s="21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A45" s="98" t="s">
-        <v>61</v>
-      </c>
-      <c r="B45" s="24">
+      <c r="B44" s="17">
         <v>1637626876.5800002</v>
       </c>
-      <c r="C45" s="25">
+      <c r="C44" s="18">
         <v>2002644803.55</v>
       </c>
-      <c r="D45" s="99">
-        <f>C45+D46+D47+D49+D50+D51+D52+D48</f>
+      <c r="D44" s="87">
+        <f>C44+D45+D46+D48+D49+D50+D51+D47</f>
         <v>2530644803.5500002</v>
       </c>
-      <c r="E45" s="99">
-        <f t="shared" ref="E45:F45" si="6">D45+E46+E47+E49+E50+E51+E52+E48</f>
+      <c r="E44" s="87">
+        <f t="shared" ref="E44:F44" si="6">D44+E45+E46+E48+E49+E50+E51+E47</f>
         <v>2880644803.5500002</v>
       </c>
-      <c r="F45" s="99">
+      <c r="F44" s="87">
         <f t="shared" si="6"/>
         <v>3230644803.5500002</v>
       </c>
-      <c r="G45" s="27"/>
-      <c r="H45" s="28"/>
-      <c r="I45" s="28"/>
-      <c r="J45" s="28"/>
-      <c r="K45" s="28"/>
-    </row>
-    <row r="46" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="A46" s="40"/>
-      <c r="B46" s="24"/>
-      <c r="C46" s="25"/>
-      <c r="D46" s="100">
+      <c r="G44" s="20"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="21"/>
+      <c r="J44" s="21"/>
+      <c r="K44" s="21"/>
+    </row>
+    <row r="45" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="33"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="88">
         <v>528000000</v>
       </c>
-      <c r="E46" s="100">
+      <c r="E45" s="88">
         <v>350000000</v>
       </c>
-      <c r="F46" s="100">
+      <c r="F45" s="88">
         <v>350000000</v>
       </c>
-      <c r="G46" s="27" t="s">
+      <c r="G45" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="H45" s="89"/>
+      <c r="I45" s="89"/>
+      <c r="J45" s="89"/>
+      <c r="K45" s="89"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A46" s="33"/>
+      <c r="B46" s="17"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="90">
+        <f>IF([1]Paramètres!$B$12=1,-D45,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E46" s="90">
+        <f>IF([1]Paramètres!$B$12=1,-E45,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F46" s="90">
+        <f>IF([1]Paramètres!$B$12=1,-F45,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G46" s="91" t="s">
+        <v>31</v>
+      </c>
+      <c r="H46" s="92"/>
+      <c r="I46" s="92"/>
+      <c r="J46" s="92"/>
+      <c r="K46" s="92"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A47" s="33"/>
+      <c r="B47" s="17"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="90">
+        <f>IF([1]Paramètres!$B$12=1,-D57,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E47" s="90"/>
+      <c r="F47" s="90"/>
+      <c r="G47" s="91" t="s">
+        <v>60</v>
+      </c>
+      <c r="H47" s="92"/>
+      <c r="I47" s="92"/>
+      <c r="J47" s="92"/>
+      <c r="K47" s="92"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A48" s="33"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="90">
+        <f>D16*[1]Paramètres!$H$7</f>
+        <v>0</v>
+      </c>
+      <c r="E48" s="90">
+        <f>E16*[1]Paramètres!$H$7</f>
+        <v>0</v>
+      </c>
+      <c r="F48" s="90">
+        <f>F16*[1]Paramètres!$H$7</f>
+        <v>0</v>
+      </c>
+      <c r="G48" s="91" t="s">
         <v>32</v>
       </c>
-      <c r="H46" s="101"/>
-      <c r="I46" s="101"/>
-      <c r="J46" s="101"/>
-      <c r="K46" s="101"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A47" s="40"/>
-      <c r="B47" s="24"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="102">
-        <f>IF([1]Paramètres!$B$12=1,-D46,0)</f>
-        <v>0</v>
-      </c>
-      <c r="E47" s="102">
-        <f>IF([1]Paramètres!$B$12=1,-E46,0)</f>
-        <v>0</v>
-      </c>
-      <c r="F47" s="102">
-        <f>IF([1]Paramètres!$B$12=1,-F46,0)</f>
-        <v>0</v>
-      </c>
-      <c r="G47" s="103" t="s">
-        <v>33</v>
-      </c>
-      <c r="H47" s="104"/>
-      <c r="I47" s="104"/>
-      <c r="J47" s="104"/>
-      <c r="K47" s="104"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A48" s="40"/>
-      <c r="B48" s="24"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="102">
-        <f>IF([1]Paramètres!$B$12=1,-D58,0)</f>
-        <v>0</v>
-      </c>
-      <c r="E48" s="102"/>
-      <c r="F48" s="102"/>
-      <c r="G48" s="103" t="s">
+      <c r="H48" s="92"/>
+      <c r="I48" s="92"/>
+      <c r="J48" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="K48" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="H48" s="104"/>
-      <c r="I48" s="104"/>
-      <c r="J48" s="104"/>
-      <c r="K48" s="104"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A49" s="40"/>
-      <c r="B49" s="24"/>
-      <c r="C49" s="25"/>
-      <c r="D49" s="102">
-        <f>D17*[1]Paramètres!$H$7</f>
-        <v>0</v>
-      </c>
-      <c r="E49" s="102">
-        <f>E17*[1]Paramètres!$H$7</f>
-        <v>0</v>
-      </c>
-      <c r="F49" s="102">
-        <f>F17*[1]Paramètres!$H$7</f>
-        <v>0</v>
-      </c>
-      <c r="G49" s="103" t="s">
-        <v>34</v>
-      </c>
-      <c r="H49" s="104"/>
-      <c r="I49" s="104"/>
-      <c r="J49" s="68" t="s">
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A49" s="33"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="90">
+        <f>-($C$44*[1]Paramètres!$E$12)/3</f>
+        <v>0</v>
+      </c>
+      <c r="E49" s="90">
+        <f>-($C$44*[1]Paramètres!$E$12)/3</f>
+        <v>0</v>
+      </c>
+      <c r="F49" s="90">
+        <f>-($C$44*[1]Paramètres!$E$12)/3</f>
+        <v>0</v>
+      </c>
+      <c r="G49" s="91" t="s">
+        <v>27</v>
+      </c>
+      <c r="H49" s="92"/>
+      <c r="I49" s="92"/>
+      <c r="J49" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="K49" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="L49" s="54"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A50" s="33"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="90">
+        <f>SUM(D23:D24)</f>
+        <v>0</v>
+      </c>
+      <c r="E50" s="90">
+        <f t="shared" ref="E50:F50" si="7">SUM(E23:E24)</f>
+        <v>0</v>
+      </c>
+      <c r="F50" s="90">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G50" s="91" t="s">
         <v>63</v>
       </c>
-      <c r="K49" s="68" t="s">
+      <c r="H50" s="92"/>
+      <c r="I50" s="92"/>
+      <c r="J50" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="K50" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="L50" s="54"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A51" s="16"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="90">
+        <f>D27</f>
+        <v>0</v>
+      </c>
+      <c r="E51" s="90">
+        <f t="shared" ref="E51:F51" si="8">E27</f>
+        <v>0</v>
+      </c>
+      <c r="F51" s="90">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G51" s="91" t="s">
+        <v>43</v>
+      </c>
+      <c r="H51" s="92"/>
+      <c r="I51" s="92"/>
+      <c r="J51" s="57"/>
+      <c r="K51" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="L51" s="54"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A52" s="41" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A50" s="40"/>
-      <c r="B50" s="24"/>
-      <c r="C50" s="25"/>
-      <c r="D50" s="102">
-        <f>-($C$45*[1]Paramètres!$E$12)/3</f>
-        <v>0</v>
-      </c>
-      <c r="E50" s="102">
-        <f>-($C$45*[1]Paramètres!$E$12)/3</f>
-        <v>0</v>
-      </c>
-      <c r="F50" s="102">
-        <f>-($C$45*[1]Paramètres!$E$12)/3</f>
-        <v>0</v>
-      </c>
-      <c r="G50" s="103" t="s">
-        <v>27</v>
-      </c>
-      <c r="H50" s="104"/>
-      <c r="I50" s="104"/>
-      <c r="J50" s="68" t="s">
-        <v>63</v>
-      </c>
-      <c r="K50" s="68" t="s">
-        <v>64</v>
-      </c>
-      <c r="L50" s="64"/>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A51" s="40"/>
-      <c r="B51" s="24"/>
-      <c r="C51" s="25"/>
-      <c r="D51" s="102">
-        <f>SUM(D24:D25)</f>
-        <v>0</v>
-      </c>
-      <c r="E51" s="102">
-        <f t="shared" ref="E51:F51" si="7">SUM(E24:E25)</f>
-        <v>0</v>
-      </c>
-      <c r="F51" s="102">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G51" s="103" t="s">
+      <c r="B52" s="17">
+        <v>6077685223.1600046</v>
+      </c>
+      <c r="C52" s="18">
+        <v>5114994327.96</v>
+      </c>
+      <c r="D52" s="87">
+        <f>C52+D53+D54+D55</f>
+        <v>5233994327.96</v>
+      </c>
+      <c r="E52" s="87">
+        <f>D52+E53+E54+E55</f>
+        <v>5288994327.9599991</v>
+      </c>
+      <c r="F52" s="87">
+        <f>E52+F53+F54+F55</f>
+        <v>5343994327.9599991</v>
+      </c>
+      <c r="G52" s="20"/>
+      <c r="H52" s="21"/>
+      <c r="I52" s="21"/>
+      <c r="J52" s="21"/>
+      <c r="K52" s="21"/>
+      <c r="L52" s="54"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A53" s="33"/>
+      <c r="B53" s="17"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="88">
+        <v>119000000</v>
+      </c>
+      <c r="E53" s="88">
+        <v>54999999.999999046</v>
+      </c>
+      <c r="F53" s="88">
+        <v>55000000</v>
+      </c>
+      <c r="G53" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="H51" s="104"/>
-      <c r="I51" s="104"/>
-      <c r="J51" s="68" t="s">
-        <v>63</v>
-      </c>
-      <c r="K51" s="68" t="s">
-        <v>64</v>
-      </c>
-      <c r="L51" s="64"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A52" s="23"/>
-      <c r="B52" s="24"/>
-      <c r="C52" s="25"/>
-      <c r="D52" s="102">
-        <f>D28</f>
-        <v>0</v>
-      </c>
-      <c r="E52" s="102">
-        <f t="shared" ref="E52:F52" si="8">E28</f>
-        <v>0</v>
-      </c>
-      <c r="F52" s="102">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="G52" s="103" t="s">
-        <v>45</v>
-      </c>
-      <c r="H52" s="104"/>
-      <c r="I52" s="104"/>
-      <c r="J52" s="68"/>
-      <c r="K52" s="68" t="s">
-        <v>64</v>
-      </c>
-      <c r="L52" s="64"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A53" s="49" t="s">
+      <c r="H53" s="89"/>
+      <c r="I53" s="21"/>
+      <c r="J53" s="89"/>
+      <c r="K53" s="89"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A54" s="33"/>
+      <c r="B54" s="17"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="90">
+        <f>IF([1]Paramètres!$B$12=1,-D53,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E54" s="90">
+        <f>IF([1]Paramètres!$B$12=1,-E53,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F54" s="90">
+        <f>IF([1]Paramètres!$B$12=1,-F53,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G54" s="91" t="s">
         <v>66</v>
       </c>
-      <c r="B53" s="24">
-        <v>6077685223.1600046</v>
-      </c>
-      <c r="C53" s="25">
-        <v>5114994327.96</v>
-      </c>
-      <c r="D53" s="99">
-        <f>C53+D54+D55+D56</f>
-        <v>5233994327.96</v>
-      </c>
-      <c r="E53" s="99">
-        <f>D53+E54+E55+E56</f>
-        <v>5288994327.9599991</v>
-      </c>
-      <c r="F53" s="99">
-        <f>E53+F54+F55+F56</f>
-        <v>5343994327.9599991</v>
-      </c>
-      <c r="G53" s="27"/>
-      <c r="H53" s="28"/>
-      <c r="I53" s="28"/>
-      <c r="J53" s="28"/>
-      <c r="K53" s="28"/>
-      <c r="L53" s="64"/>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A54" s="40"/>
-      <c r="B54" s="24"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="100">
-        <v>119000000</v>
-      </c>
-      <c r="E54" s="100">
-        <v>54999999.999999046</v>
-      </c>
-      <c r="F54" s="100">
-        <v>55000000</v>
-      </c>
-      <c r="G54" s="27" t="s">
+      <c r="H54" s="92"/>
+      <c r="I54" s="57"/>
+      <c r="J54" s="92"/>
+      <c r="K54" s="92"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A55" s="38"/>
+      <c r="B55" s="17"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="90">
+        <f>-($C$52*[1]Paramètres!$B$3)</f>
+        <v>0</v>
+      </c>
+      <c r="E55" s="90">
+        <v>0</v>
+      </c>
+      <c r="F55" s="90">
+        <v>0</v>
+      </c>
+      <c r="G55" s="91" t="s">
         <v>67</v>
       </c>
-      <c r="H54" s="101"/>
-      <c r="I54" s="28"/>
-      <c r="J54" s="101"/>
-      <c r="K54" s="101"/>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A55" s="40"/>
-      <c r="B55" s="24"/>
-      <c r="C55" s="25"/>
-      <c r="D55" s="102">
-        <f>IF([1]Paramètres!$B$12=1,-D54,0)</f>
-        <v>0</v>
-      </c>
-      <c r="E55" s="102">
-        <f>IF([1]Paramètres!$B$12=1,-E54,0)</f>
-        <v>0</v>
-      </c>
-      <c r="F55" s="102">
-        <f>IF([1]Paramètres!$B$12=1,-F54,0)</f>
-        <v>0</v>
-      </c>
-      <c r="G55" s="103" t="s">
+      <c r="H55" s="92"/>
+      <c r="I55" s="32"/>
+      <c r="J55" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="K55" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="L55" s="54"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A56" s="93" t="s">
         <v>68</v>
       </c>
-      <c r="H55" s="104"/>
-      <c r="I55" s="68"/>
-      <c r="J55" s="104"/>
-      <c r="K55" s="104"/>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A56" s="45"/>
-      <c r="B56" s="24"/>
-      <c r="C56" s="25"/>
-      <c r="D56" s="102">
-        <f>-($C$53*[1]Paramètres!$B$3)</f>
-        <v>0</v>
-      </c>
-      <c r="E56" s="102">
-        <v>0</v>
-      </c>
-      <c r="F56" s="102">
-        <v>0</v>
-      </c>
-      <c r="G56" s="103" t="s">
+      <c r="B56" s="18">
+        <v>229346258.24000001</v>
+      </c>
+      <c r="C56" s="18">
+        <v>372044704.18000001</v>
+      </c>
+      <c r="D56" s="87">
+        <f>C56+D57</f>
+        <v>152044704.18000001</v>
+      </c>
+      <c r="E56" s="87">
+        <f>D56+E57</f>
+        <v>152044704.18000001</v>
+      </c>
+      <c r="F56" s="87">
+        <f>E56+F57</f>
+        <v>152044704.18000001</v>
+      </c>
+      <c r="G56" s="50"/>
+      <c r="H56" s="51"/>
+      <c r="I56" s="51"/>
+      <c r="J56" s="51"/>
+      <c r="K56" s="51"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A57" s="94"/>
+      <c r="B57" s="18"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="88">
+        <v>-220000000</v>
+      </c>
+      <c r="E57" s="95"/>
+      <c r="F57" s="95"/>
+      <c r="G57" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="H56" s="104"/>
-      <c r="I56" s="39"/>
-      <c r="J56" s="68" t="s">
-        <v>63</v>
-      </c>
-      <c r="K56" s="68" t="s">
-        <v>64</v>
-      </c>
-      <c r="L56" s="64"/>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A57" s="105" t="s">
+      <c r="H57" s="89"/>
+      <c r="I57" s="89"/>
+      <c r="J57" s="89"/>
+      <c r="K57" s="89"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A58" s="96" t="s">
         <v>70</v>
       </c>
-      <c r="B57" s="25">
-        <v>229346258.24000001</v>
-      </c>
-      <c r="C57" s="25">
-        <v>372044704.18000001</v>
-      </c>
-      <c r="D57" s="99">
-        <f>C57+D58</f>
-        <v>152044704.18000001</v>
-      </c>
-      <c r="E57" s="99">
-        <f>D57+E58</f>
-        <v>152044704.18000001</v>
-      </c>
-      <c r="F57" s="99">
-        <f>E57+F58</f>
-        <v>152044704.18000001</v>
-      </c>
-      <c r="G57" s="58"/>
-      <c r="H57" s="59"/>
-      <c r="I57" s="59"/>
-      <c r="J57" s="59"/>
-      <c r="K57" s="59"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A58" s="106"/>
-      <c r="B58" s="25"/>
-      <c r="C58" s="25"/>
-      <c r="D58" s="100">
-        <v>-220000000</v>
-      </c>
-      <c r="E58" s="107"/>
-      <c r="F58" s="107"/>
-      <c r="G58" s="27" t="s">
+      <c r="B58" s="18">
+        <v>37413790.840000011</v>
+      </c>
+      <c r="C58" s="18"/>
+      <c r="D58" s="95"/>
+      <c r="E58" s="95"/>
+      <c r="F58" s="95"/>
+      <c r="G58" s="97"/>
+      <c r="H58" s="21"/>
+      <c r="I58" s="21"/>
+      <c r="J58" s="21"/>
+      <c r="K58" s="21"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A59" s="98"/>
+      <c r="B59" s="18"/>
+      <c r="C59" s="99"/>
+      <c r="D59" s="100"/>
+      <c r="E59" s="100"/>
+      <c r="F59" s="101"/>
+      <c r="G59" s="50"/>
+      <c r="H59" s="102"/>
+      <c r="I59" s="51"/>
+      <c r="J59" s="51"/>
+      <c r="K59" s="51"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A60" s="96" t="s">
         <v>71</v>
       </c>
-      <c r="H58" s="101"/>
-      <c r="I58" s="101"/>
-      <c r="J58" s="101"/>
-      <c r="K58" s="101"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A59" s="108" t="s">
-        <v>72</v>
-      </c>
-      <c r="B59" s="25">
-        <v>37413790.840000011</v>
-      </c>
-      <c r="C59" s="25"/>
-      <c r="D59" s="107"/>
-      <c r="E59" s="107"/>
-      <c r="F59" s="107"/>
-      <c r="G59" s="109"/>
-      <c r="H59" s="28"/>
-      <c r="I59" s="28"/>
-      <c r="J59" s="28"/>
-      <c r="K59" s="28"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A60" s="110"/>
-      <c r="B60" s="25"/>
-      <c r="C60" s="111"/>
-      <c r="D60" s="112"/>
-      <c r="E60" s="112"/>
-      <c r="F60" s="113"/>
-      <c r="G60" s="58"/>
-      <c r="H60" s="114"/>
-      <c r="I60" s="59"/>
-      <c r="J60" s="59"/>
-      <c r="K60" s="59"/>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A61" s="108" t="s">
-        <v>73</v>
-      </c>
-      <c r="B61" s="25">
+      <c r="B60" s="18">
         <v>22205607.579999998</v>
       </c>
-      <c r="C61" s="111">
+      <c r="C60" s="99">
         <v>34826910.169999994</v>
       </c>
-      <c r="D61" s="115">
-        <f>$C$61</f>
+      <c r="D60" s="103">
+        <f>$C$60</f>
         <v>34826910.169999994</v>
       </c>
-      <c r="E61" s="115">
-        <f t="shared" ref="E61:F61" si="9">$C$61</f>
+      <c r="E60" s="103">
+        <f t="shared" ref="E60:F60" si="9">$C$60</f>
         <v>34826910.169999994</v>
       </c>
-      <c r="F61" s="116">
+      <c r="F60" s="104">
         <f t="shared" si="9"/>
         <v>34826910.169999994</v>
       </c>
-      <c r="G61" s="117"/>
-      <c r="H61" s="114"/>
-      <c r="I61" s="59"/>
-      <c r="J61" s="59"/>
-      <c r="K61" s="59"/>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A62" s="118" t="s">
+      <c r="G60" s="105"/>
+      <c r="H60" s="102"/>
+      <c r="I60" s="51"/>
+      <c r="J60" s="51"/>
+      <c r="K60" s="51"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A61" s="106" t="s">
+        <v>72</v>
+      </c>
+      <c r="B61" s="18">
+        <v>111110000</v>
+      </c>
+      <c r="C61" s="158">
+        <v>759921031.86000597</v>
+      </c>
+      <c r="D61" s="161">
+        <f>C61+D65+D66</f>
+        <v>813921031.86000597</v>
+      </c>
+      <c r="E61" s="161">
+        <f>D61+E65+E66</f>
+        <v>879921031.86000597</v>
+      </c>
+      <c r="F61" s="162">
+        <f>E61+F65+F66</f>
+        <v>932921031.86000597</v>
+      </c>
+      <c r="G61" s="147"/>
+      <c r="H61" s="107"/>
+      <c r="I61" s="108"/>
+      <c r="J61" s="108"/>
+      <c r="K61" s="108"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A62" s="106" t="s">
+        <v>73</v>
+      </c>
+      <c r="B62" s="18">
+        <v>4573470.5199999996</v>
+      </c>
+      <c r="C62" s="159"/>
+      <c r="D62" s="161"/>
+      <c r="E62" s="161"/>
+      <c r="F62" s="162"/>
+      <c r="G62" s="147"/>
+      <c r="H62" s="107"/>
+      <c r="I62" s="108"/>
+      <c r="J62" s="108"/>
+      <c r="K62" s="108"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A63" s="62" t="s">
         <v>74</v>
       </c>
-      <c r="B62" s="25">
-        <v>111110000</v>
-      </c>
-      <c r="C62" s="119">
-        <v>759921031.86000597</v>
-      </c>
-      <c r="D62" s="120">
-        <f>C62+D66+D67</f>
-        <v>813921031.86000597</v>
-      </c>
-      <c r="E62" s="120">
-        <f>D62+E66+E67</f>
-        <v>879921031.86000597</v>
-      </c>
-      <c r="F62" s="121">
-        <f>E62+F66+F67</f>
-        <v>932921031.86000597</v>
-      </c>
-      <c r="G62" s="122"/>
-      <c r="H62" s="123"/>
-      <c r="I62" s="124"/>
-      <c r="J62" s="124"/>
-      <c r="K62" s="124"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A63" s="118" t="s">
+      <c r="B63" s="18">
+        <v>907655303.3499999</v>
+      </c>
+      <c r="C63" s="159"/>
+      <c r="D63" s="161"/>
+      <c r="E63" s="161"/>
+      <c r="F63" s="162"/>
+      <c r="G63" s="147"/>
+      <c r="H63" s="109"/>
+      <c r="I63" s="110"/>
+      <c r="J63" s="110"/>
+      <c r="K63" s="110"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A64" s="62" t="s">
         <v>75</v>
       </c>
-      <c r="B63" s="25">
-        <v>4573470.5199999996</v>
-      </c>
-      <c r="C63" s="125"/>
-      <c r="D63" s="120"/>
-      <c r="E63" s="120"/>
-      <c r="F63" s="121"/>
-      <c r="G63" s="122"/>
-      <c r="H63" s="123"/>
-      <c r="I63" s="124"/>
-      <c r="J63" s="124"/>
-      <c r="K63" s="124"/>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A64" s="73" t="s">
+      <c r="B64" s="99">
+        <v>495</v>
+      </c>
+      <c r="C64" s="160"/>
+      <c r="D64" s="161"/>
+      <c r="E64" s="161"/>
+      <c r="F64" s="162"/>
+      <c r="G64" s="147"/>
+      <c r="H64" s="111"/>
+      <c r="I64" s="112"/>
+      <c r="J64" s="112"/>
+      <c r="K64" s="112"/>
+    </row>
+    <row r="65" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="113"/>
+      <c r="B65" s="114"/>
+      <c r="C65" s="115"/>
+      <c r="D65" s="116">
+        <v>54000000</v>
+      </c>
+      <c r="E65" s="116">
+        <v>66000000</v>
+      </c>
+      <c r="F65" s="116">
+        <v>53000000</v>
+      </c>
+      <c r="G65" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="B64" s="25">
-        <v>907655303.3499999</v>
-      </c>
-      <c r="C64" s="125"/>
-      <c r="D64" s="120"/>
-      <c r="E64" s="120"/>
-      <c r="F64" s="121"/>
-      <c r="G64" s="122"/>
-      <c r="H64" s="126"/>
-      <c r="I64" s="127"/>
-      <c r="J64" s="127"/>
-      <c r="K64" s="127"/>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A65" s="73" t="s">
+      <c r="H65" s="117"/>
+      <c r="I65" s="117"/>
+      <c r="J65" s="117"/>
+      <c r="K65" s="117"/>
+    </row>
+    <row r="66" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="62"/>
+      <c r="B66" s="18"/>
+      <c r="C66" s="18"/>
+      <c r="D66" s="35">
+        <f>IF([1]Paramètres!$B$12=1,-D65,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E66" s="35">
+        <f>IF([1]Paramètres!$B$12=1,-E65,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F66" s="35">
+        <f>IF([1]Paramètres!$B$12=1,-F65,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G66" s="91" t="s">
         <v>77</v>
       </c>
-      <c r="B65" s="111">
-        <v>495</v>
-      </c>
-      <c r="C65" s="128"/>
-      <c r="D65" s="120"/>
-      <c r="E65" s="120"/>
-      <c r="F65" s="121"/>
-      <c r="G65" s="122"/>
-      <c r="H65" s="129"/>
-      <c r="I65" s="130"/>
-      <c r="J65" s="130"/>
-      <c r="K65" s="130"/>
-    </row>
-    <row r="66" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="131"/>
-      <c r="B66" s="132"/>
-      <c r="C66" s="133"/>
-      <c r="D66" s="134">
-        <v>54000000</v>
-      </c>
-      <c r="E66" s="134">
-        <v>66000000</v>
-      </c>
-      <c r="F66" s="134">
-        <v>53000000</v>
-      </c>
-      <c r="G66" s="27" t="s">
+      <c r="H66" s="92"/>
+      <c r="I66" s="92"/>
+      <c r="J66" s="92"/>
+      <c r="K66" s="92"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A67" s="118" t="s">
         <v>78</v>
       </c>
-      <c r="H66" s="135"/>
-      <c r="I66" s="135"/>
-      <c r="J66" s="135"/>
-      <c r="K66" s="135"/>
-    </row>
-    <row r="67" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="73"/>
-      <c r="B67" s="25"/>
-      <c r="C67" s="25"/>
-      <c r="D67" s="42">
-        <f>IF([1]Paramètres!$B$12=1,-D66,0)</f>
-        <v>0</v>
-      </c>
-      <c r="E67" s="42">
-        <f>IF([1]Paramètres!$B$12=1,-E66,0)</f>
-        <v>0</v>
-      </c>
-      <c r="F67" s="42">
-        <f>IF([1]Paramètres!$B$12=1,-F66,0)</f>
-        <v>0</v>
-      </c>
-      <c r="G67" s="103" t="s">
+      <c r="B67" s="80">
+        <v>29595396.759999949</v>
+      </c>
+      <c r="C67" s="119">
+        <v>53539907.449994996</v>
+      </c>
+      <c r="D67" s="120">
+        <f>C67+D69+D70+D71+D72+D73+D74+D75+D76+D77+D68</f>
+        <v>65539907.449994996</v>
+      </c>
+      <c r="E67" s="120">
+        <f>D67+E69+E70+E71+E72+E73+E74+E75+E76+E77+E68</f>
+        <v>166539907.44999498</v>
+      </c>
+      <c r="F67" s="120">
+        <f>E67+F69+F70+F71+F72+F73+F74+F75+F76+F77+F68</f>
+        <v>343539907.44999498</v>
+      </c>
+      <c r="G67" s="121"/>
+      <c r="H67" s="51"/>
+      <c r="I67" s="51"/>
+      <c r="J67" s="51"/>
+      <c r="K67" s="51"/>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A68" s="122"/>
+      <c r="B68" s="123"/>
+      <c r="C68" s="115"/>
+      <c r="D68" s="116">
+        <v>12000000</v>
+      </c>
+      <c r="E68" s="116">
+        <v>101000000</v>
+      </c>
+      <c r="F68" s="116">
+        <v>177000000</v>
+      </c>
+      <c r="G68" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="H67" s="104"/>
-      <c r="I67" s="104"/>
-      <c r="J67" s="104"/>
-      <c r="K67" s="104"/>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A68" s="136" t="s">
+      <c r="H68" s="124"/>
+      <c r="I68" s="124"/>
+      <c r="J68" s="124"/>
+      <c r="K68" s="124"/>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A69" s="122"/>
+      <c r="B69" s="123"/>
+      <c r="C69" s="115"/>
+      <c r="D69" s="35">
+        <f>IF([1]Paramètres!$B$12=1,-D68,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E69" s="35">
+        <f>IF([1]Paramètres!$B$12=1,-E68,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F69" s="35">
+        <f>IF([1]Paramètres!$B$12=1,-F68,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G69" s="91" t="s">
         <v>80</v>
       </c>
-      <c r="B68" s="92">
-        <v>29595396.759999949</v>
-      </c>
-      <c r="C68" s="137">
-        <v>53539907.449994996</v>
-      </c>
-      <c r="D68" s="138">
-        <f>C68+D70+D71+D72+D73+D74+D75+D76+D77+D78+D69</f>
-        <v>65539907.449994996</v>
-      </c>
-      <c r="E68" s="138">
-        <f>D68+E70+E71+E72+E73+E74+E75+E76+E77+E78+E69</f>
-        <v>166539907.44999498</v>
-      </c>
-      <c r="F68" s="138">
-        <f>E68+F70+F71+F72+F73+F74+F75+F76+F77+F78+F69</f>
-        <v>343539907.44999498</v>
-      </c>
-      <c r="G68" s="139"/>
-      <c r="H68" s="59"/>
-      <c r="I68" s="59"/>
-      <c r="J68" s="59"/>
-      <c r="K68" s="59"/>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A69" s="140"/>
-      <c r="B69" s="141"/>
-      <c r="C69" s="133"/>
-      <c r="D69" s="134">
-        <v>12000000</v>
-      </c>
-      <c r="E69" s="134">
-        <v>101000000</v>
-      </c>
-      <c r="F69" s="134">
-        <v>177000000</v>
-      </c>
-      <c r="G69" s="27" t="s">
+      <c r="H69" s="57"/>
+      <c r="I69" s="57"/>
+      <c r="J69" s="57"/>
+      <c r="K69" s="57"/>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A70" s="122"/>
+      <c r="B70" s="123"/>
+      <c r="C70" s="115"/>
+      <c r="D70" s="35">
+        <f>-[1]Paramètres!$B$20*[1]Paramètres!$B$21</f>
+        <v>0</v>
+      </c>
+      <c r="E70" s="35">
+        <v>0</v>
+      </c>
+      <c r="F70" s="35">
+        <v>0</v>
+      </c>
+      <c r="G70" s="91" t="s">
         <v>81</v>
       </c>
-      <c r="H69" s="142"/>
-      <c r="I69" s="142"/>
-      <c r="J69" s="142"/>
-      <c r="K69" s="142"/>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A70" s="140"/>
-      <c r="B70" s="141"/>
-      <c r="C70" s="133"/>
-      <c r="D70" s="42">
-        <f>IF([1]Paramètres!$B$12=1,-D69,0)</f>
-        <v>0</v>
-      </c>
-      <c r="E70" s="42">
-        <f>IF([1]Paramètres!$B$12=1,-E69,0)</f>
-        <v>0</v>
-      </c>
-      <c r="F70" s="42">
-        <f>IF([1]Paramètres!$B$12=1,-F69,0)</f>
-        <v>0</v>
-      </c>
-      <c r="G70" s="103" t="s">
+      <c r="H70" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="I70" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="J70" s="57"/>
+      <c r="K70" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="L70" s="125"/>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A71" s="122"/>
+      <c r="B71" s="123"/>
+      <c r="C71" s="115"/>
+      <c r="D71" s="35">
+        <f>-[1]Paramètres!$E$20*[1]Paramètres!$E$21</f>
+        <v>0</v>
+      </c>
+      <c r="E71" s="35">
+        <v>0</v>
+      </c>
+      <c r="F71" s="35"/>
+      <c r="G71" s="91" t="s">
         <v>82</v>
       </c>
-      <c r="H70" s="68"/>
-      <c r="I70" s="68"/>
-      <c r="J70" s="68"/>
-      <c r="K70" s="68"/>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A71" s="140"/>
-      <c r="B71" s="141"/>
-      <c r="C71" s="133"/>
-      <c r="D71" s="42">
-        <f>-[1]Paramètres!$B$20*[1]Paramètres!$B$21</f>
-        <v>0</v>
-      </c>
-      <c r="E71" s="42">
-        <v>0</v>
-      </c>
-      <c r="F71" s="42">
-        <v>0</v>
-      </c>
-      <c r="G71" s="103" t="s">
+      <c r="H71" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="I71" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="J71" s="57"/>
+      <c r="K71" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="L71" s="125"/>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A72" s="122"/>
+      <c r="B72" s="123"/>
+      <c r="C72" s="115"/>
+      <c r="D72" s="35">
+        <f>-[1]Paramètres!$K$12*[1]Paramètres!$K$13</f>
+        <v>0</v>
+      </c>
+      <c r="E72" s="35">
+        <v>0</v>
+      </c>
+      <c r="F72" s="35">
+        <v>0</v>
+      </c>
+      <c r="G72" s="91" t="s">
         <v>83</v>
       </c>
-      <c r="H71" s="68" t="s">
+      <c r="H72" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="I71" s="68" t="s">
+      <c r="I72" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="J71" s="68"/>
-      <c r="K71" s="68" t="s">
-        <v>64</v>
-      </c>
-      <c r="L71" s="143"/>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A72" s="140"/>
-      <c r="B72" s="141"/>
-      <c r="C72" s="133"/>
-      <c r="D72" s="42">
-        <f>-[1]Paramètres!$E$20*[1]Paramètres!$E$21</f>
-        <v>0</v>
-      </c>
-      <c r="E72" s="42">
-        <v>0</v>
-      </c>
-      <c r="F72" s="42"/>
-      <c r="G72" s="103" t="s">
+      <c r="J72" s="57"/>
+      <c r="K72" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="L72" s="125"/>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A73" s="122"/>
+      <c r="B73" s="123"/>
+      <c r="C73" s="115"/>
+      <c r="D73" s="35">
+        <f>-[1]Paramètres!$H$20*[1]Paramètres!$H$21</f>
+        <v>0</v>
+      </c>
+      <c r="E73" s="35">
+        <v>0</v>
+      </c>
+      <c r="F73" s="35"/>
+      <c r="G73" s="91" t="s">
+        <v>49</v>
+      </c>
+      <c r="H73" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="I73" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="J73" s="57"/>
+      <c r="K73" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="L73" s="125"/>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A74" s="122"/>
+      <c r="B74" s="123"/>
+      <c r="C74" s="115"/>
+      <c r="D74" s="35">
+        <f>-[1]Paramètres!$B$30*[1]Paramètres!$B$31</f>
+        <v>0</v>
+      </c>
+      <c r="E74" s="35">
+        <v>0</v>
+      </c>
+      <c r="F74" s="35"/>
+      <c r="G74" s="91" t="s">
+        <v>50</v>
+      </c>
+      <c r="H74" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="I74" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="J74" s="57"/>
+      <c r="K74" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="L74" s="125"/>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A75" s="122"/>
+      <c r="B75" s="123"/>
+      <c r="C75" s="115"/>
+      <c r="D75" s="35">
+        <f>-([1]Paramètres!$H$13*[1]Paramètres!$H$15)/3</f>
+        <v>0</v>
+      </c>
+      <c r="E75" s="35">
+        <f>-([1]Paramètres!$H$13*[1]Paramètres!$H$15)/3</f>
+        <v>0</v>
+      </c>
+      <c r="F75" s="35">
+        <f>-([1]Paramètres!$H$13*[1]Paramètres!$H$15)/3</f>
+        <v>0</v>
+      </c>
+      <c r="G75" s="91" t="s">
         <v>84</v>
       </c>
-      <c r="H72" s="68" t="s">
+      <c r="H75" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="I72" s="68" t="s">
+      <c r="I75" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="J72" s="68"/>
-      <c r="K72" s="68" t="s">
-        <v>64</v>
-      </c>
-      <c r="L72" s="143"/>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A73" s="140"/>
-      <c r="B73" s="141"/>
-      <c r="C73" s="133"/>
-      <c r="D73" s="42">
-        <f>-[1]Paramètres!$K$12*[1]Paramètres!$K$13</f>
-        <v>0</v>
-      </c>
-      <c r="E73" s="42">
-        <v>0</v>
-      </c>
-      <c r="F73" s="42">
-        <v>0</v>
-      </c>
-      <c r="G73" s="103" t="s">
+      <c r="J75" s="57"/>
+      <c r="K75" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="L75" s="125"/>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A76" s="126"/>
+      <c r="B76" s="123"/>
+      <c r="C76" s="115"/>
+      <c r="D76" s="35">
+        <f>D18</f>
+        <v>0</v>
+      </c>
+      <c r="E76" s="35"/>
+      <c r="F76" s="35"/>
+      <c r="G76" s="91" t="s">
+        <v>34</v>
+      </c>
+      <c r="H76" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="I76" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="J76" s="57"/>
+      <c r="K76" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="L76" s="125"/>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A77" s="113"/>
+      <c r="B77" s="114"/>
+      <c r="C77" s="115"/>
+      <c r="D77" s="35">
+        <f>IF([1]Paramètres!$K$20=1,[1]Paramètres!$K21,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E77" s="35">
+        <f>IF([1]Paramètres!$K$20=1,[1]Paramètres!$K22,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F77" s="35">
+        <f>IF([1]Paramètres!$K$20=1,[1]Paramètres!$K23,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G77" s="91" t="s">
+        <v>51</v>
+      </c>
+      <c r="H77" s="92" t="s">
+        <v>29</v>
+      </c>
+      <c r="I77" s="92" t="s">
+        <v>29</v>
+      </c>
+      <c r="J77" s="92"/>
+      <c r="K77" s="92"/>
+      <c r="L77" s="125"/>
+    </row>
+    <row r="78" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="127" t="s">
         <v>85</v>
       </c>
-      <c r="H73" s="68" t="s">
-        <v>29</v>
-      </c>
-      <c r="I73" s="68" t="s">
-        <v>29</v>
-      </c>
-      <c r="J73" s="68"/>
-      <c r="K73" s="68" t="s">
-        <v>64</v>
-      </c>
-      <c r="L73" s="143"/>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A74" s="140"/>
-      <c r="B74" s="141"/>
-      <c r="C74" s="133"/>
-      <c r="D74" s="42">
-        <f>-[1]Paramètres!$H$20*[1]Paramètres!$H$21</f>
-        <v>0</v>
-      </c>
-      <c r="E74" s="42">
-        <v>0</v>
-      </c>
-      <c r="F74" s="42"/>
-      <c r="G74" s="103" t="s">
-        <v>51</v>
-      </c>
-      <c r="H74" s="68" t="s">
-        <v>29</v>
-      </c>
-      <c r="I74" s="68" t="s">
-        <v>29</v>
-      </c>
-      <c r="J74" s="68"/>
-      <c r="K74" s="68" t="s">
-        <v>64</v>
-      </c>
-      <c r="L74" s="143"/>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A75" s="140"/>
-      <c r="B75" s="141"/>
-      <c r="C75" s="133"/>
-      <c r="D75" s="42">
-        <f>-[1]Paramètres!$B$30*[1]Paramètres!$B$31</f>
-        <v>0</v>
-      </c>
-      <c r="E75" s="42">
-        <v>0</v>
-      </c>
-      <c r="F75" s="42"/>
-      <c r="G75" s="103" t="s">
+      <c r="B78" s="128">
+        <f>SUM(B44:B68)</f>
+        <v>9057212422.0300045</v>
+      </c>
+      <c r="C78" s="129">
+        <v>8337971685.170002</v>
+      </c>
+      <c r="D78" s="130">
+        <f>+D44+D52+D56+D58+D60+D61+D67</f>
+        <v>8830971685.170002</v>
+      </c>
+      <c r="E78" s="130">
+        <f>+E44+E52+E56+E59+E60+E61+E67</f>
+        <v>9402971685.1700001</v>
+      </c>
+      <c r="F78" s="130">
+        <f>+F44+F52+F56+F59+F60+F61+F67</f>
+        <v>10037971685.17</v>
+      </c>
+      <c r="G78" s="131"/>
+      <c r="H78" s="21"/>
+      <c r="I78" s="21"/>
+      <c r="J78" s="21"/>
+      <c r="K78" s="21"/>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A79" s="132"/>
+      <c r="B79" s="133"/>
+      <c r="C79" s="134"/>
+      <c r="D79" s="135"/>
+      <c r="E79" s="135"/>
+      <c r="F79" s="135"/>
+      <c r="G79" s="136"/>
+      <c r="H79" s="137"/>
+      <c r="I79" s="137"/>
+      <c r="J79" s="137"/>
+      <c r="K79" s="137"/>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A80" s="98" t="s">
         <v>52</v>
       </c>
-      <c r="H75" s="68" t="s">
-        <v>29</v>
-      </c>
-      <c r="I75" s="68" t="s">
-        <v>29</v>
-      </c>
-      <c r="J75" s="68"/>
-      <c r="K75" s="68" t="s">
-        <v>64</v>
-      </c>
-      <c r="L75" s="143"/>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A76" s="140"/>
-      <c r="B76" s="141"/>
-      <c r="C76" s="133"/>
-      <c r="D76" s="42">
-        <f>-([1]Paramètres!$H$13*[1]Paramètres!$H$15)/3</f>
-        <v>0</v>
-      </c>
-      <c r="E76" s="42">
-        <f>-([1]Paramètres!$H$13*[1]Paramètres!$H$15)/3</f>
-        <v>0</v>
-      </c>
-      <c r="F76" s="42">
-        <f>-([1]Paramètres!$H$13*[1]Paramètres!$H$15)/3</f>
-        <v>0</v>
-      </c>
-      <c r="G76" s="103" t="s">
+      <c r="B80" s="18">
+        <v>1039163376.0900002</v>
+      </c>
+      <c r="C80" s="138">
+        <v>1293887720.8</v>
+      </c>
+      <c r="D80" s="81">
+        <f>C80</f>
+        <v>1293887720.8</v>
+      </c>
+      <c r="E80" s="81">
+        <f>D80</f>
+        <v>1293887720.8</v>
+      </c>
+      <c r="F80" s="81">
+        <f>E80</f>
+        <v>1293887720.8</v>
+      </c>
+      <c r="G80" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H80" s="124"/>
+      <c r="I80" s="124"/>
+      <c r="J80" s="124"/>
+      <c r="K80" s="124"/>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A81" s="83" t="s">
+        <v>57</v>
+      </c>
+      <c r="B81" s="84"/>
+      <c r="C81" s="84"/>
+      <c r="D81" s="84"/>
+      <c r="E81" s="84"/>
+      <c r="F81" s="84"/>
+      <c r="G81" s="84"/>
+      <c r="H81" s="85"/>
+      <c r="I81" s="85"/>
+      <c r="J81" s="85"/>
+      <c r="K81" s="85"/>
+    </row>
+    <row r="82" spans="1:11" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B82" s="140"/>
+      <c r="D82" s="52"/>
+      <c r="E82" s="52"/>
+      <c r="F82" s="52"/>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A83" s="142" t="s">
         <v>86</v>
       </c>
-      <c r="H76" s="68" t="s">
-        <v>29</v>
-      </c>
-      <c r="I76" s="68" t="s">
-        <v>29</v>
-      </c>
-      <c r="J76" s="68"/>
-      <c r="K76" s="68" t="s">
-        <v>64</v>
-      </c>
-      <c r="L76" s="143"/>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A77" s="144"/>
-      <c r="B77" s="141"/>
-      <c r="C77" s="133"/>
-      <c r="D77" s="42">
-        <f>D19</f>
-        <v>0</v>
-      </c>
-      <c r="E77" s="42"/>
-      <c r="F77" s="42"/>
-      <c r="G77" s="103" t="s">
-        <v>36</v>
-      </c>
-      <c r="H77" s="68" t="s">
-        <v>29</v>
-      </c>
-      <c r="I77" s="68" t="s">
-        <v>29</v>
-      </c>
-      <c r="J77" s="68"/>
-      <c r="K77" s="68" t="s">
-        <v>64</v>
-      </c>
-      <c r="L77" s="143"/>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A78" s="131"/>
-      <c r="B78" s="132"/>
-      <c r="C78" s="133"/>
-      <c r="D78" s="42">
-        <f>IF([1]Paramètres!$K$20=1,[1]Paramètres!$K21,0)</f>
-        <v>0</v>
-      </c>
-      <c r="E78" s="42">
-        <f>IF([1]Paramètres!$K$20=1,[1]Paramètres!$K22,0)</f>
-        <v>0</v>
-      </c>
-      <c r="F78" s="42">
-        <f>IF([1]Paramètres!$K$20=1,[1]Paramètres!$K23,0)</f>
-        <v>0</v>
-      </c>
-      <c r="G78" s="103" t="s">
-        <v>53</v>
-      </c>
-      <c r="H78" s="104" t="s">
-        <v>29</v>
-      </c>
-      <c r="I78" s="104" t="s">
-        <v>29</v>
-      </c>
-      <c r="J78" s="104"/>
-      <c r="K78" s="104"/>
-      <c r="L78" s="143"/>
-    </row>
-    <row r="79" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="145" t="s">
-        <v>87</v>
-      </c>
-      <c r="B79" s="146">
-        <f>SUM(B45:B69)</f>
-        <v>9057212422.0300045</v>
-      </c>
-      <c r="C79" s="147">
-        <v>8337971685.170002</v>
-      </c>
-      <c r="D79" s="148">
-        <f>+D45+D53+D57+D59+D61+D62+D68</f>
-        <v>8830971685.170002</v>
-      </c>
-      <c r="E79" s="148">
-        <f>+E45+E53+E57+E60+E61+E62+E68</f>
-        <v>9402971685.1700001</v>
-      </c>
-      <c r="F79" s="148">
-        <f>+F45+F53+F57+F60+F61+F62+F68</f>
-        <v>10037971685.17</v>
-      </c>
-      <c r="G79" s="149"/>
-      <c r="H79" s="28"/>
-      <c r="I79" s="28"/>
-      <c r="J79" s="28"/>
-      <c r="K79" s="28"/>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A80" s="150"/>
-      <c r="B80" s="151"/>
-      <c r="C80" s="152"/>
-      <c r="D80" s="153"/>
-      <c r="E80" s="153"/>
-      <c r="F80" s="153"/>
-      <c r="G80" s="154"/>
-      <c r="H80" s="155"/>
-      <c r="I80" s="155"/>
-      <c r="J80" s="155"/>
-      <c r="K80" s="155"/>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A81" s="110" t="s">
-        <v>54</v>
-      </c>
-      <c r="B81" s="25">
-        <v>1039163376.0900002</v>
-      </c>
-      <c r="C81" s="156">
-        <v>1293887720.8</v>
-      </c>
-      <c r="D81" s="93">
-        <f>C81</f>
-        <v>1293887720.8</v>
-      </c>
-      <c r="E81" s="93">
-        <f>D81</f>
-        <v>1293887720.8</v>
-      </c>
-      <c r="F81" s="93">
-        <f>E81</f>
-        <v>1293887720.8</v>
-      </c>
-      <c r="G81" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="H81" s="142"/>
-      <c r="I81" s="142"/>
-      <c r="J81" s="142"/>
-      <c r="K81" s="142"/>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A82" s="95" t="s">
-        <v>59</v>
-      </c>
-      <c r="B82" s="96"/>
-      <c r="C82" s="96"/>
-      <c r="D82" s="96"/>
-      <c r="E82" s="96"/>
-      <c r="F82" s="96"/>
-      <c r="G82" s="96"/>
-      <c r="H82" s="97"/>
-      <c r="I82" s="97"/>
-      <c r="J82" s="97"/>
-      <c r="K82" s="97"/>
-    </row>
-    <row r="83" spans="1:11" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B83" s="158"/>
-      <c r="D83" s="61"/>
-      <c r="E83" s="61"/>
-      <c r="F83" s="61"/>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A84" s="160" t="s">
-        <v>88</v>
-      </c>
-      <c r="B84" s="161">
-        <f>B79-B36</f>
-        <v>-2228683.3900032043</v>
-      </c>
-      <c r="C84" s="161">
-        <f>C79-C36</f>
+      <c r="B83" s="143">
+        <f>B78-B35</f>
+        <v>2072739722.2899981</v>
+      </c>
+      <c r="C83" s="143">
+        <f>C78-C35</f>
         <v>113188.68000221252</v>
       </c>
-      <c r="D84" s="161">
-        <f>D79-D36</f>
+      <c r="D83" s="143">
+        <f>D78-D35</f>
         <v>113188.68000221252</v>
       </c>
-      <c r="E84" s="161">
-        <f>E79-E36</f>
+      <c r="E83" s="143">
+        <f>E78-E35</f>
         <v>113188.68000030518</v>
       </c>
-      <c r="F84" s="161">
-        <f>F79-F36</f>
+      <c r="F83" s="143">
+        <f>F78-F35</f>
         <v>113188.68000030518</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="D85" s="162"/>
-      <c r="E85" s="162"/>
-      <c r="F85" s="162"/>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C86" s="61"/>
-      <c r="D86" s="163"/>
-      <c r="E86" s="163"/>
-      <c r="F86" s="163"/>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="D87" s="61"/>
-      <c r="E87" s="61"/>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C89" s="61"/>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D84" s="144"/>
+      <c r="E84" s="144"/>
+      <c r="F84" s="144"/>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C85" s="52"/>
+      <c r="D85" s="145"/>
+      <c r="E85" s="145"/>
+      <c r="F85" s="145"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D86" s="52"/>
+      <c r="E86" s="52"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C88" s="52"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A21:A28"/>
-    <mergeCell ref="C62:C65"/>
-    <mergeCell ref="D62:D65"/>
-    <mergeCell ref="E62:E65"/>
-    <mergeCell ref="F62:F65"/>
-    <mergeCell ref="G62:G65"/>
+  <mergeCells count="10">
+    <mergeCell ref="G61:G64"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="A20:A27"/>
+    <mergeCell ref="C61:C64"/>
+    <mergeCell ref="D61:D64"/>
+    <mergeCell ref="E61:E64"/>
+    <mergeCell ref="F61:F64"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>